<commit_message>
Actualizando lista de frases de preguntas administrativas, acomodando logs, aplicando análisis de presición de generación y procesamiento de preguntas y respuestas
</commit_message>
<xml_diff>
--- a/docs/Analisis_de_resultados/analisis_14_05_25/Analisis_muestreo_14_05_25.xlsx
+++ b/docs/Analisis_de_resultados/analisis_14_05_25/Analisis_muestreo_14_05_25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\Análisis_de_resultados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\python_con_json\obtener_preguntas_y_respuestas\docs\Analisis_de_resultados\analisis_22_05_25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633D8FE5-76AE-4329-80FD-99C3793AAEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E112461-7251-4D6D-9F0B-33672759F0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="5" r:id="rId1"/>
@@ -320,21 +320,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> es el tamaño de la muestra (ej. 188 preguntas).</t>
-    </r>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -345,7 +330,7 @@
   </si>
   <si>
     <r>
-      <t>En el JSON 1 analicé 63 preguntas, me dio 84% respondidas. Como el margen de error es ±5.24%, el valor real podría estar entre 78,76</t>
+      <t xml:space="preserve">En el JSON 1 analicé 63 preguntas, me dio 84% respondidas. Como el margen de error es ±9.05%, el valor real podría estar entre 75,08 </t>
     </r>
     <r>
       <rPr>
@@ -356,7 +341,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>% y 89,24%</t>
+      <t>% y 93,05%</t>
     </r>
     <r>
       <rPr>
@@ -371,7 +356,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">En el JSON 2 analicé 52  preguntas, me dio 77% respondidas. Como el margen de error es ±6.63%, el valor real podría estar entre 70,37% y 83,63 </t>
+      <t xml:space="preserve">En el JSON 2 analicé 52  preguntas, me dio 77% respondidas. Como el margen de error es ±6.63%, el valor real podría estar entre 65,48% y 88,36 </t>
     </r>
     <r>
       <rPr>
@@ -397,7 +382,7 @@
   </si>
   <si>
     <r>
-      <t>En el JSON 3 analicé 46  preguntas, me dio 85% respondidas. Como el margen de error es ±5.98%, el valor real podría estar entre 79,02% y  90,98</t>
+      <t>En el JSON 3 analicé 46  preguntas, me dio 85% respondidas. Como el margen de error es ±5.98%, el valor real podría estar entre 74,46% y  95,10</t>
     </r>
     <r>
       <rPr>
@@ -419,6 +404,21 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es el tamaño de la muestra (ej. 63 preguntas).</t>
     </r>
   </si>
 </sst>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AA836D-385C-4141-AF5A-AAFCA35CFBC3}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,7 +898,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -910,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A2C344-2C27-4DA7-86CE-E96FF95C17C2}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
@@ -2284,12 +2284,12 @@
       </c>
       <c r="B72" s="2">
         <f>B73*(B74*(1-B74)/B75)^(1/2)</f>
-        <v>5.2405489399002241E-2</v>
+        <v>9.0528522208933329E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73">
         <v>1.96</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="4">
         <v>0.84</v>
@@ -2305,19 +2305,20 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75">
-        <v>188</v>
+        <f>A66</f>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D64" xr:uid="{087FBB79-01BD-4E4B-ADDE-6AD6AD213152}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
@@ -2330,7 +2331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CC5732-B338-44B3-8D97-F14A8D822F6E}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
@@ -3498,12 +3499,12 @@
       </c>
       <c r="B62" s="2">
         <f>B63*(B64*(1-B64)/B65)^(1/2)</f>
-        <v>6.6252077751958932E-2</v>
+        <v>0.11438357870307729</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B63">
         <v>1.96</v>
@@ -3511,7 +3512,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B64" s="4">
         <v>0.77</v>
@@ -3519,15 +3520,16 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65">
-        <v>155</v>
+        <f>A55</f>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3544,8 +3546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639649E8-2E8A-40E0-BC08-8A4E79862374}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4608,12 +4610,12 @@
       </c>
       <c r="B56" s="2">
         <f>B57*(B58*(1-B58)/B59)^(1/2)</f>
-        <v>5.979307383662523E-2</v>
+        <v>0.10318872536996598</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B57">
         <v>1.96</v>
@@ -4621,7 +4623,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58" s="4">
         <v>0.85</v>
@@ -4629,15 +4631,16 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B59">
-        <v>137</v>
+        <f>A49</f>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>